<commit_message>
ok 78.5,add interact file
</commit_message>
<xml_diff>
--- a/NOTE/new words.xlsx
+++ b/NOTE/new words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11491" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11771" uniqueCount="760">
   <si>
     <t>inner: ben trong</t>
   </si>
@@ -2298,6 +2298,12 @@
   </si>
   <si>
     <t>receipt  bien lai</t>
+  </si>
+  <si>
+    <t>affect anh huong den</t>
+  </si>
+  <si>
+    <t>difinitely chac chan</t>
   </si>
 </sst>
 </file>
@@ -2685,8 +2691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V670"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="A235" sqref="A235"/>
+    <sheetView tabSelected="1" topLeftCell="P225" workbookViewId="0">
+      <selection activeCell="U244" sqref="U244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15613,6 +15619,874 @@
         <v>225</v>
       </c>
       <c r="T229" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>227</v>
+      </c>
+      <c r="B231" t="s">
+        <v>211</v>
+      </c>
+      <c r="C231" t="s">
+        <v>31</v>
+      </c>
+      <c r="D231" t="s">
+        <v>212</v>
+      </c>
+      <c r="E231" t="s">
+        <v>213</v>
+      </c>
+      <c r="F231" t="s">
+        <v>35</v>
+      </c>
+      <c r="G231" t="s">
+        <v>214</v>
+      </c>
+      <c r="H231" t="s">
+        <v>215</v>
+      </c>
+      <c r="I231" t="s">
+        <v>216</v>
+      </c>
+      <c r="J231" t="s">
+        <v>217</v>
+      </c>
+      <c r="K231" t="s">
+        <v>218</v>
+      </c>
+      <c r="L231" t="s">
+        <v>36</v>
+      </c>
+      <c r="M231" t="s">
+        <v>219</v>
+      </c>
+      <c r="N231" t="s">
+        <v>220</v>
+      </c>
+      <c r="O231" t="s">
+        <v>221</v>
+      </c>
+      <c r="P231" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q231" t="s">
+        <v>758</v>
+      </c>
+      <c r="R231" t="s">
+        <v>224</v>
+      </c>
+      <c r="S231" t="s">
+        <v>759</v>
+      </c>
+      <c r="T231" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>227</v>
+      </c>
+      <c r="B232" t="s">
+        <v>211</v>
+      </c>
+      <c r="C232" t="s">
+        <v>31</v>
+      </c>
+      <c r="D232" t="s">
+        <v>212</v>
+      </c>
+      <c r="E232" t="s">
+        <v>213</v>
+      </c>
+      <c r="F232" t="s">
+        <v>35</v>
+      </c>
+      <c r="G232" t="s">
+        <v>214</v>
+      </c>
+      <c r="H232" t="s">
+        <v>215</v>
+      </c>
+      <c r="I232" t="s">
+        <v>216</v>
+      </c>
+      <c r="J232" t="s">
+        <v>217</v>
+      </c>
+      <c r="K232" t="s">
+        <v>218</v>
+      </c>
+      <c r="L232" t="s">
+        <v>36</v>
+      </c>
+      <c r="M232" t="s">
+        <v>219</v>
+      </c>
+      <c r="N232" t="s">
+        <v>220</v>
+      </c>
+      <c r="O232" t="s">
+        <v>221</v>
+      </c>
+      <c r="P232" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q232" t="s">
+        <v>758</v>
+      </c>
+      <c r="R232" t="s">
+        <v>224</v>
+      </c>
+      <c r="S232" t="s">
+        <v>759</v>
+      </c>
+      <c r="T232" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>227</v>
+      </c>
+      <c r="B233" t="s">
+        <v>211</v>
+      </c>
+      <c r="C233" t="s">
+        <v>31</v>
+      </c>
+      <c r="D233" t="s">
+        <v>212</v>
+      </c>
+      <c r="E233" t="s">
+        <v>213</v>
+      </c>
+      <c r="F233" t="s">
+        <v>35</v>
+      </c>
+      <c r="G233" t="s">
+        <v>214</v>
+      </c>
+      <c r="H233" t="s">
+        <v>215</v>
+      </c>
+      <c r="I233" t="s">
+        <v>216</v>
+      </c>
+      <c r="J233" t="s">
+        <v>217</v>
+      </c>
+      <c r="K233" t="s">
+        <v>218</v>
+      </c>
+      <c r="L233" t="s">
+        <v>36</v>
+      </c>
+      <c r="M233" t="s">
+        <v>219</v>
+      </c>
+      <c r="N233" t="s">
+        <v>220</v>
+      </c>
+      <c r="O233" t="s">
+        <v>221</v>
+      </c>
+      <c r="P233" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q233" t="s">
+        <v>758</v>
+      </c>
+      <c r="R233" t="s">
+        <v>224</v>
+      </c>
+      <c r="S233" t="s">
+        <v>759</v>
+      </c>
+      <c r="T233" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>227</v>
+      </c>
+      <c r="B234" t="s">
+        <v>211</v>
+      </c>
+      <c r="C234" t="s">
+        <v>31</v>
+      </c>
+      <c r="D234" t="s">
+        <v>212</v>
+      </c>
+      <c r="E234" t="s">
+        <v>213</v>
+      </c>
+      <c r="F234" t="s">
+        <v>35</v>
+      </c>
+      <c r="G234" t="s">
+        <v>214</v>
+      </c>
+      <c r="H234" t="s">
+        <v>215</v>
+      </c>
+      <c r="I234" t="s">
+        <v>216</v>
+      </c>
+      <c r="J234" t="s">
+        <v>217</v>
+      </c>
+      <c r="K234" t="s">
+        <v>218</v>
+      </c>
+      <c r="L234" t="s">
+        <v>36</v>
+      </c>
+      <c r="M234" t="s">
+        <v>219</v>
+      </c>
+      <c r="N234" t="s">
+        <v>220</v>
+      </c>
+      <c r="O234" t="s">
+        <v>221</v>
+      </c>
+      <c r="P234" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q234" t="s">
+        <v>758</v>
+      </c>
+      <c r="R234" t="s">
+        <v>224</v>
+      </c>
+      <c r="S234" t="s">
+        <v>759</v>
+      </c>
+      <c r="T234" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>227</v>
+      </c>
+      <c r="B235" t="s">
+        <v>211</v>
+      </c>
+      <c r="C235" t="s">
+        <v>31</v>
+      </c>
+      <c r="D235" t="s">
+        <v>212</v>
+      </c>
+      <c r="E235" t="s">
+        <v>213</v>
+      </c>
+      <c r="F235" t="s">
+        <v>35</v>
+      </c>
+      <c r="G235" t="s">
+        <v>214</v>
+      </c>
+      <c r="H235" t="s">
+        <v>215</v>
+      </c>
+      <c r="I235" t="s">
+        <v>216</v>
+      </c>
+      <c r="J235" t="s">
+        <v>217</v>
+      </c>
+      <c r="K235" t="s">
+        <v>218</v>
+      </c>
+      <c r="L235" t="s">
+        <v>36</v>
+      </c>
+      <c r="M235" t="s">
+        <v>219</v>
+      </c>
+      <c r="N235" t="s">
+        <v>220</v>
+      </c>
+      <c r="O235" t="s">
+        <v>221</v>
+      </c>
+      <c r="P235" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q235" t="s">
+        <v>758</v>
+      </c>
+      <c r="R235" t="s">
+        <v>224</v>
+      </c>
+      <c r="S235" t="s">
+        <v>759</v>
+      </c>
+      <c r="T235" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>227</v>
+      </c>
+      <c r="B236" t="s">
+        <v>211</v>
+      </c>
+      <c r="C236" t="s">
+        <v>31</v>
+      </c>
+      <c r="D236" t="s">
+        <v>212</v>
+      </c>
+      <c r="E236" t="s">
+        <v>213</v>
+      </c>
+      <c r="F236" t="s">
+        <v>35</v>
+      </c>
+      <c r="G236" t="s">
+        <v>214</v>
+      </c>
+      <c r="H236" t="s">
+        <v>215</v>
+      </c>
+      <c r="I236" t="s">
+        <v>216</v>
+      </c>
+      <c r="J236" t="s">
+        <v>217</v>
+      </c>
+      <c r="K236" t="s">
+        <v>218</v>
+      </c>
+      <c r="L236" t="s">
+        <v>36</v>
+      </c>
+      <c r="M236" t="s">
+        <v>219</v>
+      </c>
+      <c r="N236" t="s">
+        <v>220</v>
+      </c>
+      <c r="O236" t="s">
+        <v>221</v>
+      </c>
+      <c r="P236" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q236" t="s">
+        <v>758</v>
+      </c>
+      <c r="R236" t="s">
+        <v>224</v>
+      </c>
+      <c r="S236" t="s">
+        <v>759</v>
+      </c>
+      <c r="T236" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>227</v>
+      </c>
+      <c r="B237" t="s">
+        <v>211</v>
+      </c>
+      <c r="C237" t="s">
+        <v>31</v>
+      </c>
+      <c r="D237" t="s">
+        <v>212</v>
+      </c>
+      <c r="E237" t="s">
+        <v>213</v>
+      </c>
+      <c r="F237" t="s">
+        <v>35</v>
+      </c>
+      <c r="G237" t="s">
+        <v>214</v>
+      </c>
+      <c r="H237" t="s">
+        <v>215</v>
+      </c>
+      <c r="I237" t="s">
+        <v>216</v>
+      </c>
+      <c r="J237" t="s">
+        <v>217</v>
+      </c>
+      <c r="K237" t="s">
+        <v>218</v>
+      </c>
+      <c r="L237" t="s">
+        <v>36</v>
+      </c>
+      <c r="M237" t="s">
+        <v>219</v>
+      </c>
+      <c r="N237" t="s">
+        <v>220</v>
+      </c>
+      <c r="O237" t="s">
+        <v>221</v>
+      </c>
+      <c r="P237" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q237" t="s">
+        <v>758</v>
+      </c>
+      <c r="R237" t="s">
+        <v>224</v>
+      </c>
+      <c r="S237" t="s">
+        <v>759</v>
+      </c>
+      <c r="T237" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>227</v>
+      </c>
+      <c r="B238" t="s">
+        <v>211</v>
+      </c>
+      <c r="C238" t="s">
+        <v>31</v>
+      </c>
+      <c r="D238" t="s">
+        <v>212</v>
+      </c>
+      <c r="E238" t="s">
+        <v>213</v>
+      </c>
+      <c r="F238" t="s">
+        <v>35</v>
+      </c>
+      <c r="G238" t="s">
+        <v>214</v>
+      </c>
+      <c r="H238" t="s">
+        <v>215</v>
+      </c>
+      <c r="I238" t="s">
+        <v>216</v>
+      </c>
+      <c r="J238" t="s">
+        <v>217</v>
+      </c>
+      <c r="K238" t="s">
+        <v>218</v>
+      </c>
+      <c r="L238" t="s">
+        <v>36</v>
+      </c>
+      <c r="M238" t="s">
+        <v>219</v>
+      </c>
+      <c r="N238" t="s">
+        <v>220</v>
+      </c>
+      <c r="O238" t="s">
+        <v>221</v>
+      </c>
+      <c r="P238" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q238" t="s">
+        <v>758</v>
+      </c>
+      <c r="R238" t="s">
+        <v>224</v>
+      </c>
+      <c r="S238" t="s">
+        <v>759</v>
+      </c>
+      <c r="T238" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>227</v>
+      </c>
+      <c r="B239" t="s">
+        <v>211</v>
+      </c>
+      <c r="C239" t="s">
+        <v>31</v>
+      </c>
+      <c r="D239" t="s">
+        <v>212</v>
+      </c>
+      <c r="E239" t="s">
+        <v>213</v>
+      </c>
+      <c r="F239" t="s">
+        <v>35</v>
+      </c>
+      <c r="G239" t="s">
+        <v>214</v>
+      </c>
+      <c r="H239" t="s">
+        <v>215</v>
+      </c>
+      <c r="I239" t="s">
+        <v>216</v>
+      </c>
+      <c r="J239" t="s">
+        <v>217</v>
+      </c>
+      <c r="K239" t="s">
+        <v>218</v>
+      </c>
+      <c r="L239" t="s">
+        <v>36</v>
+      </c>
+      <c r="M239" t="s">
+        <v>219</v>
+      </c>
+      <c r="N239" t="s">
+        <v>220</v>
+      </c>
+      <c r="O239" t="s">
+        <v>221</v>
+      </c>
+      <c r="P239" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q239" t="s">
+        <v>758</v>
+      </c>
+      <c r="R239" t="s">
+        <v>224</v>
+      </c>
+      <c r="S239" t="s">
+        <v>759</v>
+      </c>
+      <c r="T239" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>227</v>
+      </c>
+      <c r="B240" t="s">
+        <v>211</v>
+      </c>
+      <c r="C240" t="s">
+        <v>31</v>
+      </c>
+      <c r="D240" t="s">
+        <v>212</v>
+      </c>
+      <c r="E240" t="s">
+        <v>213</v>
+      </c>
+      <c r="F240" t="s">
+        <v>35</v>
+      </c>
+      <c r="G240" t="s">
+        <v>214</v>
+      </c>
+      <c r="H240" t="s">
+        <v>215</v>
+      </c>
+      <c r="I240" t="s">
+        <v>216</v>
+      </c>
+      <c r="J240" t="s">
+        <v>217</v>
+      </c>
+      <c r="K240" t="s">
+        <v>218</v>
+      </c>
+      <c r="L240" t="s">
+        <v>36</v>
+      </c>
+      <c r="M240" t="s">
+        <v>219</v>
+      </c>
+      <c r="N240" t="s">
+        <v>220</v>
+      </c>
+      <c r="O240" t="s">
+        <v>221</v>
+      </c>
+      <c r="P240" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q240" t="s">
+        <v>758</v>
+      </c>
+      <c r="R240" t="s">
+        <v>224</v>
+      </c>
+      <c r="S240" t="s">
+        <v>759</v>
+      </c>
+      <c r="T240" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>227</v>
+      </c>
+      <c r="B241" t="s">
+        <v>211</v>
+      </c>
+      <c r="C241" t="s">
+        <v>31</v>
+      </c>
+      <c r="D241" t="s">
+        <v>212</v>
+      </c>
+      <c r="E241" t="s">
+        <v>213</v>
+      </c>
+      <c r="F241" t="s">
+        <v>35</v>
+      </c>
+      <c r="G241" t="s">
+        <v>214</v>
+      </c>
+      <c r="H241" t="s">
+        <v>215</v>
+      </c>
+      <c r="I241" t="s">
+        <v>216</v>
+      </c>
+      <c r="J241" t="s">
+        <v>217</v>
+      </c>
+      <c r="K241" t="s">
+        <v>218</v>
+      </c>
+      <c r="L241" t="s">
+        <v>36</v>
+      </c>
+      <c r="M241" t="s">
+        <v>219</v>
+      </c>
+      <c r="N241" t="s">
+        <v>220</v>
+      </c>
+      <c r="O241" t="s">
+        <v>221</v>
+      </c>
+      <c r="P241" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q241" t="s">
+        <v>758</v>
+      </c>
+      <c r="R241" t="s">
+        <v>224</v>
+      </c>
+      <c r="S241" t="s">
+        <v>759</v>
+      </c>
+      <c r="T241" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>227</v>
+      </c>
+      <c r="B242" t="s">
+        <v>211</v>
+      </c>
+      <c r="C242" t="s">
+        <v>31</v>
+      </c>
+      <c r="D242" t="s">
+        <v>212</v>
+      </c>
+      <c r="E242" t="s">
+        <v>213</v>
+      </c>
+      <c r="F242" t="s">
+        <v>35</v>
+      </c>
+      <c r="G242" t="s">
+        <v>214</v>
+      </c>
+      <c r="H242" t="s">
+        <v>215</v>
+      </c>
+      <c r="I242" t="s">
+        <v>216</v>
+      </c>
+      <c r="J242" t="s">
+        <v>217</v>
+      </c>
+      <c r="K242" t="s">
+        <v>218</v>
+      </c>
+      <c r="L242" t="s">
+        <v>36</v>
+      </c>
+      <c r="M242" t="s">
+        <v>219</v>
+      </c>
+      <c r="N242" t="s">
+        <v>220</v>
+      </c>
+      <c r="O242" t="s">
+        <v>221</v>
+      </c>
+      <c r="P242" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q242" t="s">
+        <v>758</v>
+      </c>
+      <c r="R242" t="s">
+        <v>224</v>
+      </c>
+      <c r="S242" t="s">
+        <v>759</v>
+      </c>
+      <c r="T242" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>227</v>
+      </c>
+      <c r="B243" t="s">
+        <v>211</v>
+      </c>
+      <c r="C243" t="s">
+        <v>31</v>
+      </c>
+      <c r="D243" t="s">
+        <v>212</v>
+      </c>
+      <c r="E243" t="s">
+        <v>213</v>
+      </c>
+      <c r="F243" t="s">
+        <v>35</v>
+      </c>
+      <c r="G243" t="s">
+        <v>214</v>
+      </c>
+      <c r="H243" t="s">
+        <v>215</v>
+      </c>
+      <c r="I243" t="s">
+        <v>216</v>
+      </c>
+      <c r="J243" t="s">
+        <v>217</v>
+      </c>
+      <c r="K243" t="s">
+        <v>218</v>
+      </c>
+      <c r="L243" t="s">
+        <v>36</v>
+      </c>
+      <c r="M243" t="s">
+        <v>219</v>
+      </c>
+      <c r="N243" t="s">
+        <v>220</v>
+      </c>
+      <c r="O243" t="s">
+        <v>221</v>
+      </c>
+      <c r="P243" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q243" t="s">
+        <v>758</v>
+      </c>
+      <c r="R243" t="s">
+        <v>224</v>
+      </c>
+      <c r="S243" t="s">
+        <v>759</v>
+      </c>
+      <c r="T243" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>227</v>
+      </c>
+      <c r="B244" t="s">
+        <v>211</v>
+      </c>
+      <c r="C244" t="s">
+        <v>31</v>
+      </c>
+      <c r="D244" t="s">
+        <v>212</v>
+      </c>
+      <c r="E244" t="s">
+        <v>213</v>
+      </c>
+      <c r="F244" t="s">
+        <v>35</v>
+      </c>
+      <c r="G244" t="s">
+        <v>214</v>
+      </c>
+      <c r="H244" t="s">
+        <v>215</v>
+      </c>
+      <c r="I244" t="s">
+        <v>216</v>
+      </c>
+      <c r="J244" t="s">
+        <v>217</v>
+      </c>
+      <c r="K244" t="s">
+        <v>218</v>
+      </c>
+      <c r="L244" t="s">
+        <v>36</v>
+      </c>
+      <c r="M244" t="s">
+        <v>219</v>
+      </c>
+      <c r="N244" t="s">
+        <v>220</v>
+      </c>
+      <c r="O244" t="s">
+        <v>221</v>
+      </c>
+      <c r="P244" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q244" t="s">
+        <v>758</v>
+      </c>
+      <c r="R244" t="s">
+        <v>224</v>
+      </c>
+      <c r="S244" t="s">
+        <v>759</v>
+      </c>
+      <c r="T244" t="s">
         <v>226</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add 43 sap xep tong hop CTDL-GT
</commit_message>
<xml_diff>
--- a/NOTE/new words.xlsx
+++ b/NOTE/new words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15621" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16176" uniqueCount="806">
   <si>
     <t>inner: ben trong</t>
   </si>
@@ -2301,6 +2301,147 @@
   </si>
   <si>
     <t xml:space="preserve">accord phu hop tan thanh </t>
+  </si>
+  <si>
+    <t>identified: xac dinh</t>
+  </si>
+  <si>
+    <t>Enhance: nang cao</t>
+  </si>
+  <si>
+    <t>Cohesive: ket hop,ket dinh</t>
+  </si>
+  <si>
+    <t>31 decimal: thap phan</t>
+  </si>
+  <si>
+    <t>27 subtract: phep tru</t>
+  </si>
+  <si>
+    <t>depth: chieu sau,do sau</t>
+  </si>
+  <si>
+    <t>redundant du thua ko can thiet</t>
+  </si>
+  <si>
+    <t>Redundant: du thua,ko can thiet</t>
+  </si>
+  <si>
+    <t>enhance nang cao</t>
+  </si>
+  <si>
+    <t>cohesive ket hop ket dinh</t>
+  </si>
+  <si>
+    <t>decimal thap phan</t>
+  </si>
+  <si>
+    <t>subtract phep tru</t>
+  </si>
+  <si>
+    <t>depth chieu sau do sau</t>
+  </si>
+  <si>
+    <t>ability kha nang</t>
+  </si>
+  <si>
+    <t>access truy cap</t>
+  </si>
+  <si>
+    <t>analyst nha phan tich</t>
+  </si>
+  <si>
+    <t>centerpiece manh trung tam</t>
+  </si>
+  <si>
+    <t>equipment thiet bi</t>
+  </si>
+  <si>
+    <t>interact tuong tac</t>
+  </si>
+  <si>
+    <t>reliability co the tin cay</t>
+  </si>
+  <si>
+    <t>activity hoat dong</t>
+  </si>
+  <si>
+    <t>animation hoat hinh</t>
+  </si>
+  <si>
+    <t>coordinate phoi hop</t>
+  </si>
+  <si>
+    <t>distribute phan phoi</t>
+  </si>
+  <si>
+    <t>divide phan chia</t>
+  </si>
+  <si>
+    <t>estimate uoc luong</t>
+  </si>
+  <si>
+    <t>interchange trao doi lan nhau</t>
+  </si>
+  <si>
+    <t>liquid chat long</t>
+  </si>
+  <si>
+    <t>encode ma hoa</t>
+  </si>
+  <si>
+    <t>expertise thanh thao</t>
+  </si>
+  <si>
+    <t>majority phan lon</t>
+  </si>
+  <si>
+    <t>solve giai quyet</t>
+  </si>
+  <si>
+    <t>superior cao hon phia tren</t>
+  </si>
+  <si>
+    <t>sophistication phuc tap</t>
+  </si>
+  <si>
+    <t>contemporary cung luc dong thoi</t>
+  </si>
+  <si>
+    <t>disparate khac nhau</t>
+  </si>
+  <si>
+    <t>encourage dong vien khuyen khich</t>
+  </si>
+  <si>
+    <t>discourage ko dong vien</t>
+  </si>
+  <si>
+    <t>essential thiet yeu can ban</t>
+  </si>
+  <si>
+    <t>potential tiem nang</t>
+  </si>
+  <si>
+    <t>predict tien doan du doan</t>
+  </si>
+  <si>
+    <t>resume khoi phuc</t>
+  </si>
+  <si>
+    <t>semiconductor ban dan</t>
+  </si>
+  <si>
+    <t>indicate chi ra cho biet</t>
+  </si>
+  <si>
+    <t>immense bao la rong lon</t>
+  </si>
+  <si>
+    <t>imitate mo phong</t>
+  </si>
+  <si>
+    <t>filtration loc</t>
   </si>
 </sst>
 </file>
@@ -2686,10 +2827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V880"/>
+  <dimension ref="A1:V914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P861" workbookViewId="0">
-      <selection activeCell="T880" sqref="T880"/>
+    <sheetView tabSelected="1" topLeftCell="P898" workbookViewId="0">
+      <selection activeCell="U911" sqref="U911"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51197,6 +51338,1727 @@
       </c>
       <c r="T880" t="s">
         <v>749</v>
+      </c>
+    </row>
+    <row r="883" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A883" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B883" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="C883" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="D883" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="E883" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="F883" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="G883" t="s">
+        <v>764</v>
+      </c>
+      <c r="H883" t="s">
+        <v>599</v>
+      </c>
+      <c r="I883" t="s">
+        <v>690</v>
+      </c>
+      <c r="J883" t="s">
+        <v>687</v>
+      </c>
+      <c r="K883" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="L883" t="s">
+        <v>215</v>
+      </c>
+      <c r="M883" t="s">
+        <v>491</v>
+      </c>
+      <c r="N883" t="s">
+        <v>490</v>
+      </c>
+      <c r="O883" t="s">
+        <v>186</v>
+      </c>
+      <c r="P883" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q883" t="s">
+        <v>40</v>
+      </c>
+      <c r="R883" t="s">
+        <v>34</v>
+      </c>
+      <c r="S883" t="s">
+        <v>136</v>
+      </c>
+      <c r="T883" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="884" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>219</v>
+      </c>
+      <c r="B884" t="s">
+        <v>765</v>
+      </c>
+      <c r="C884" t="s">
+        <v>767</v>
+      </c>
+      <c r="D884" t="s">
+        <v>768</v>
+      </c>
+      <c r="E884" t="s">
+        <v>769</v>
+      </c>
+      <c r="F884" t="s">
+        <v>770</v>
+      </c>
+      <c r="G884" t="s">
+        <v>771</v>
+      </c>
+      <c r="H884" t="s">
+        <v>599</v>
+      </c>
+      <c r="I884" t="s">
+        <v>690</v>
+      </c>
+      <c r="J884" t="s">
+        <v>687</v>
+      </c>
+      <c r="K884" t="s">
+        <v>636</v>
+      </c>
+      <c r="L884" t="s">
+        <v>215</v>
+      </c>
+      <c r="M884" t="s">
+        <v>491</v>
+      </c>
+      <c r="N884" t="s">
+        <v>490</v>
+      </c>
+      <c r="O884" t="s">
+        <v>186</v>
+      </c>
+      <c r="P884" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q884" t="s">
+        <v>25</v>
+      </c>
+      <c r="R884" t="s">
+        <v>34</v>
+      </c>
+      <c r="S884" t="s">
+        <v>136</v>
+      </c>
+      <c r="T884" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="885" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>219</v>
+      </c>
+      <c r="B885" t="s">
+        <v>765</v>
+      </c>
+      <c r="C885" t="s">
+        <v>767</v>
+      </c>
+      <c r="D885" t="s">
+        <v>768</v>
+      </c>
+      <c r="E885" t="s">
+        <v>769</v>
+      </c>
+      <c r="F885" t="s">
+        <v>770</v>
+      </c>
+      <c r="G885" t="s">
+        <v>771</v>
+      </c>
+      <c r="H885" t="s">
+        <v>599</v>
+      </c>
+      <c r="I885" t="s">
+        <v>690</v>
+      </c>
+      <c r="J885" t="s">
+        <v>687</v>
+      </c>
+      <c r="K885" t="s">
+        <v>636</v>
+      </c>
+      <c r="L885" t="s">
+        <v>215</v>
+      </c>
+      <c r="M885" t="s">
+        <v>491</v>
+      </c>
+      <c r="N885" t="s">
+        <v>490</v>
+      </c>
+      <c r="O885" t="s">
+        <v>186</v>
+      </c>
+      <c r="P885" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q885" t="s">
+        <v>25</v>
+      </c>
+      <c r="R885" t="s">
+        <v>34</v>
+      </c>
+      <c r="S885" t="s">
+        <v>136</v>
+      </c>
+      <c r="T885" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="886" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>219</v>
+      </c>
+      <c r="B886" t="s">
+        <v>765</v>
+      </c>
+      <c r="C886" t="s">
+        <v>767</v>
+      </c>
+      <c r="D886" t="s">
+        <v>768</v>
+      </c>
+      <c r="E886" t="s">
+        <v>769</v>
+      </c>
+      <c r="F886" t="s">
+        <v>770</v>
+      </c>
+      <c r="G886" t="s">
+        <v>771</v>
+      </c>
+      <c r="H886" t="s">
+        <v>599</v>
+      </c>
+      <c r="I886" t="s">
+        <v>690</v>
+      </c>
+      <c r="J886" t="s">
+        <v>687</v>
+      </c>
+      <c r="K886" t="s">
+        <v>636</v>
+      </c>
+      <c r="L886" t="s">
+        <v>215</v>
+      </c>
+      <c r="M886" t="s">
+        <v>491</v>
+      </c>
+      <c r="N886" t="s">
+        <v>490</v>
+      </c>
+      <c r="O886" t="s">
+        <v>186</v>
+      </c>
+      <c r="P886" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q886" t="s">
+        <v>25</v>
+      </c>
+      <c r="R886" t="s">
+        <v>34</v>
+      </c>
+      <c r="S886" t="s">
+        <v>136</v>
+      </c>
+      <c r="T886" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="887" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>219</v>
+      </c>
+      <c r="B887" t="s">
+        <v>765</v>
+      </c>
+      <c r="C887" t="s">
+        <v>767</v>
+      </c>
+      <c r="D887" t="s">
+        <v>768</v>
+      </c>
+      <c r="E887" t="s">
+        <v>769</v>
+      </c>
+      <c r="F887" t="s">
+        <v>770</v>
+      </c>
+      <c r="G887" t="s">
+        <v>771</v>
+      </c>
+      <c r="H887" t="s">
+        <v>599</v>
+      </c>
+      <c r="I887" t="s">
+        <v>690</v>
+      </c>
+      <c r="J887" t="s">
+        <v>687</v>
+      </c>
+      <c r="K887" t="s">
+        <v>636</v>
+      </c>
+      <c r="L887" t="s">
+        <v>215</v>
+      </c>
+      <c r="M887" t="s">
+        <v>491</v>
+      </c>
+      <c r="N887" t="s">
+        <v>490</v>
+      </c>
+      <c r="O887" t="s">
+        <v>186</v>
+      </c>
+      <c r="P887" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q887" t="s">
+        <v>25</v>
+      </c>
+      <c r="R887" t="s">
+        <v>34</v>
+      </c>
+      <c r="S887" t="s">
+        <v>136</v>
+      </c>
+      <c r="T887" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="888" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>219</v>
+      </c>
+      <c r="B888" t="s">
+        <v>765</v>
+      </c>
+      <c r="C888" t="s">
+        <v>767</v>
+      </c>
+      <c r="D888" t="s">
+        <v>768</v>
+      </c>
+      <c r="E888" t="s">
+        <v>769</v>
+      </c>
+      <c r="F888" t="s">
+        <v>770</v>
+      </c>
+      <c r="G888" t="s">
+        <v>771</v>
+      </c>
+      <c r="H888" t="s">
+        <v>599</v>
+      </c>
+      <c r="I888" t="s">
+        <v>690</v>
+      </c>
+      <c r="J888" t="s">
+        <v>687</v>
+      </c>
+      <c r="K888" t="s">
+        <v>636</v>
+      </c>
+      <c r="L888" t="s">
+        <v>215</v>
+      </c>
+      <c r="M888" t="s">
+        <v>491</v>
+      </c>
+      <c r="N888" t="s">
+        <v>490</v>
+      </c>
+      <c r="O888" t="s">
+        <v>186</v>
+      </c>
+      <c r="P888" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q888" t="s">
+        <v>25</v>
+      </c>
+      <c r="R888" t="s">
+        <v>34</v>
+      </c>
+      <c r="S888" t="s">
+        <v>136</v>
+      </c>
+      <c r="T888" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="889" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>219</v>
+      </c>
+      <c r="B889" t="s">
+        <v>765</v>
+      </c>
+      <c r="C889" t="s">
+        <v>767</v>
+      </c>
+      <c r="D889" t="s">
+        <v>768</v>
+      </c>
+      <c r="E889" t="s">
+        <v>769</v>
+      </c>
+      <c r="F889" t="s">
+        <v>770</v>
+      </c>
+      <c r="G889" t="s">
+        <v>771</v>
+      </c>
+      <c r="H889" t="s">
+        <v>599</v>
+      </c>
+      <c r="I889" t="s">
+        <v>690</v>
+      </c>
+      <c r="J889" t="s">
+        <v>687</v>
+      </c>
+      <c r="K889" t="s">
+        <v>636</v>
+      </c>
+      <c r="L889" t="s">
+        <v>215</v>
+      </c>
+      <c r="M889" t="s">
+        <v>491</v>
+      </c>
+      <c r="N889" t="s">
+        <v>490</v>
+      </c>
+      <c r="O889" t="s">
+        <v>186</v>
+      </c>
+      <c r="P889" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q889" t="s">
+        <v>25</v>
+      </c>
+      <c r="R889" t="s">
+        <v>34</v>
+      </c>
+      <c r="S889" t="s">
+        <v>136</v>
+      </c>
+      <c r="T889" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="890" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>219</v>
+      </c>
+      <c r="B890" t="s">
+        <v>765</v>
+      </c>
+      <c r="C890" t="s">
+        <v>767</v>
+      </c>
+      <c r="D890" t="s">
+        <v>768</v>
+      </c>
+      <c r="E890" t="s">
+        <v>769</v>
+      </c>
+      <c r="F890" t="s">
+        <v>770</v>
+      </c>
+      <c r="G890" t="s">
+        <v>771</v>
+      </c>
+      <c r="H890" t="s">
+        <v>599</v>
+      </c>
+      <c r="I890" t="s">
+        <v>690</v>
+      </c>
+      <c r="J890" t="s">
+        <v>687</v>
+      </c>
+      <c r="K890" t="s">
+        <v>636</v>
+      </c>
+      <c r="L890" t="s">
+        <v>215</v>
+      </c>
+      <c r="M890" t="s">
+        <v>491</v>
+      </c>
+      <c r="N890" t="s">
+        <v>490</v>
+      </c>
+      <c r="O890" t="s">
+        <v>186</v>
+      </c>
+      <c r="P890" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q890" t="s">
+        <v>25</v>
+      </c>
+      <c r="R890" t="s">
+        <v>34</v>
+      </c>
+      <c r="S890" t="s">
+        <v>136</v>
+      </c>
+      <c r="T890" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="891" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>219</v>
+      </c>
+      <c r="B891" t="s">
+        <v>765</v>
+      </c>
+      <c r="C891" t="s">
+        <v>767</v>
+      </c>
+      <c r="D891" t="s">
+        <v>768</v>
+      </c>
+      <c r="E891" t="s">
+        <v>769</v>
+      </c>
+      <c r="F891" t="s">
+        <v>770</v>
+      </c>
+      <c r="G891" t="s">
+        <v>771</v>
+      </c>
+      <c r="H891" t="s">
+        <v>599</v>
+      </c>
+      <c r="I891" t="s">
+        <v>690</v>
+      </c>
+      <c r="J891" t="s">
+        <v>687</v>
+      </c>
+      <c r="K891" t="s">
+        <v>636</v>
+      </c>
+      <c r="L891" t="s">
+        <v>215</v>
+      </c>
+      <c r="M891" t="s">
+        <v>491</v>
+      </c>
+      <c r="N891" t="s">
+        <v>490</v>
+      </c>
+      <c r="O891" t="s">
+        <v>186</v>
+      </c>
+      <c r="P891" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q891" t="s">
+        <v>25</v>
+      </c>
+      <c r="R891" t="s">
+        <v>34</v>
+      </c>
+      <c r="S891" t="s">
+        <v>136</v>
+      </c>
+      <c r="T891" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="892" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>219</v>
+      </c>
+      <c r="B892" t="s">
+        <v>765</v>
+      </c>
+      <c r="C892" t="s">
+        <v>767</v>
+      </c>
+      <c r="D892" t="s">
+        <v>768</v>
+      </c>
+      <c r="E892" t="s">
+        <v>769</v>
+      </c>
+      <c r="F892" t="s">
+        <v>770</v>
+      </c>
+      <c r="G892" t="s">
+        <v>771</v>
+      </c>
+      <c r="H892" t="s">
+        <v>599</v>
+      </c>
+      <c r="I892" t="s">
+        <v>690</v>
+      </c>
+      <c r="J892" t="s">
+        <v>687</v>
+      </c>
+      <c r="K892" t="s">
+        <v>636</v>
+      </c>
+      <c r="L892" t="s">
+        <v>215</v>
+      </c>
+      <c r="M892" t="s">
+        <v>491</v>
+      </c>
+      <c r="N892" t="s">
+        <v>490</v>
+      </c>
+      <c r="O892" t="s">
+        <v>186</v>
+      </c>
+      <c r="P892" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q892" t="s">
+        <v>25</v>
+      </c>
+      <c r="R892" t="s">
+        <v>34</v>
+      </c>
+      <c r="S892" t="s">
+        <v>136</v>
+      </c>
+      <c r="T892" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="893" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>219</v>
+      </c>
+      <c r="B893" t="s">
+        <v>765</v>
+      </c>
+      <c r="C893" t="s">
+        <v>767</v>
+      </c>
+      <c r="D893" t="s">
+        <v>768</v>
+      </c>
+      <c r="E893" t="s">
+        <v>769</v>
+      </c>
+      <c r="F893" t="s">
+        <v>770</v>
+      </c>
+      <c r="G893" t="s">
+        <v>771</v>
+      </c>
+      <c r="H893" t="s">
+        <v>599</v>
+      </c>
+      <c r="I893" t="s">
+        <v>690</v>
+      </c>
+      <c r="J893" t="s">
+        <v>687</v>
+      </c>
+      <c r="K893" t="s">
+        <v>636</v>
+      </c>
+      <c r="L893" t="s">
+        <v>215</v>
+      </c>
+      <c r="M893" t="s">
+        <v>491</v>
+      </c>
+      <c r="N893" t="s">
+        <v>490</v>
+      </c>
+      <c r="O893" t="s">
+        <v>186</v>
+      </c>
+      <c r="P893" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q893" t="s">
+        <v>25</v>
+      </c>
+      <c r="R893" t="s">
+        <v>34</v>
+      </c>
+      <c r="S893" t="s">
+        <v>136</v>
+      </c>
+      <c r="T893" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="894" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>219</v>
+      </c>
+      <c r="B894" t="s">
+        <v>765</v>
+      </c>
+      <c r="C894" t="s">
+        <v>767</v>
+      </c>
+      <c r="D894" t="s">
+        <v>768</v>
+      </c>
+      <c r="E894" t="s">
+        <v>769</v>
+      </c>
+      <c r="F894" t="s">
+        <v>770</v>
+      </c>
+      <c r="G894" t="s">
+        <v>771</v>
+      </c>
+      <c r="H894" t="s">
+        <v>599</v>
+      </c>
+      <c r="I894" t="s">
+        <v>690</v>
+      </c>
+      <c r="J894" t="s">
+        <v>687</v>
+      </c>
+      <c r="K894" t="s">
+        <v>636</v>
+      </c>
+      <c r="L894" t="s">
+        <v>215</v>
+      </c>
+      <c r="M894" t="s">
+        <v>491</v>
+      </c>
+      <c r="N894" t="s">
+        <v>490</v>
+      </c>
+      <c r="O894" t="s">
+        <v>186</v>
+      </c>
+      <c r="P894" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q894" t="s">
+        <v>25</v>
+      </c>
+      <c r="R894" t="s">
+        <v>34</v>
+      </c>
+      <c r="S894" t="s">
+        <v>136</v>
+      </c>
+      <c r="T894" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="895" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>219</v>
+      </c>
+      <c r="B895" t="s">
+        <v>765</v>
+      </c>
+      <c r="C895" t="s">
+        <v>767</v>
+      </c>
+      <c r="D895" t="s">
+        <v>768</v>
+      </c>
+      <c r="E895" t="s">
+        <v>769</v>
+      </c>
+      <c r="F895" t="s">
+        <v>770</v>
+      </c>
+      <c r="G895" t="s">
+        <v>771</v>
+      </c>
+      <c r="H895" t="s">
+        <v>599</v>
+      </c>
+      <c r="I895" t="s">
+        <v>690</v>
+      </c>
+      <c r="J895" t="s">
+        <v>687</v>
+      </c>
+      <c r="K895" t="s">
+        <v>636</v>
+      </c>
+      <c r="L895" t="s">
+        <v>215</v>
+      </c>
+      <c r="M895" t="s">
+        <v>491</v>
+      </c>
+      <c r="N895" t="s">
+        <v>490</v>
+      </c>
+      <c r="O895" t="s">
+        <v>186</v>
+      </c>
+      <c r="P895" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q895" t="s">
+        <v>25</v>
+      </c>
+      <c r="R895" t="s">
+        <v>34</v>
+      </c>
+      <c r="S895" t="s">
+        <v>136</v>
+      </c>
+      <c r="T895" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="896" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>219</v>
+      </c>
+      <c r="B896" t="s">
+        <v>765</v>
+      </c>
+      <c r="C896" t="s">
+        <v>767</v>
+      </c>
+      <c r="D896" t="s">
+        <v>768</v>
+      </c>
+      <c r="E896" t="s">
+        <v>769</v>
+      </c>
+      <c r="F896" t="s">
+        <v>770</v>
+      </c>
+      <c r="G896" t="s">
+        <v>771</v>
+      </c>
+      <c r="H896" t="s">
+        <v>599</v>
+      </c>
+      <c r="I896" t="s">
+        <v>690</v>
+      </c>
+      <c r="J896" t="s">
+        <v>687</v>
+      </c>
+      <c r="K896" t="s">
+        <v>636</v>
+      </c>
+      <c r="L896" t="s">
+        <v>215</v>
+      </c>
+      <c r="M896" t="s">
+        <v>491</v>
+      </c>
+      <c r="N896" t="s">
+        <v>490</v>
+      </c>
+      <c r="O896" t="s">
+        <v>186</v>
+      </c>
+      <c r="P896" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q896" t="s">
+        <v>25</v>
+      </c>
+      <c r="R896" t="s">
+        <v>34</v>
+      </c>
+      <c r="S896" t="s">
+        <v>136</v>
+      </c>
+      <c r="T896" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="899" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>772</v>
+      </c>
+      <c r="B899" t="s">
+        <v>773</v>
+      </c>
+      <c r="C899" t="s">
+        <v>774</v>
+      </c>
+      <c r="D899" t="s">
+        <v>775</v>
+      </c>
+      <c r="E899" t="s">
+        <v>776</v>
+      </c>
+      <c r="F899" t="s">
+        <v>777</v>
+      </c>
+      <c r="G899" t="s">
+        <v>778</v>
+      </c>
+      <c r="H899" t="s">
+        <v>779</v>
+      </c>
+      <c r="I899" t="s">
+        <v>780</v>
+      </c>
+      <c r="J899" t="s">
+        <v>781</v>
+      </c>
+      <c r="K899" t="s">
+        <v>427</v>
+      </c>
+      <c r="L899" t="s">
+        <v>782</v>
+      </c>
+      <c r="M899" t="s">
+        <v>783</v>
+      </c>
+      <c r="N899" t="s">
+        <v>784</v>
+      </c>
+      <c r="O899" t="s">
+        <v>785</v>
+      </c>
+      <c r="P899" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q899" t="s">
+        <v>787</v>
+      </c>
+      <c r="R899" t="s">
+        <v>788</v>
+      </c>
+      <c r="S899" t="s">
+        <v>789</v>
+      </c>
+      <c r="T899" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="900" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
+        <v>772</v>
+      </c>
+      <c r="B900" t="s">
+        <v>773</v>
+      </c>
+      <c r="C900" t="s">
+        <v>774</v>
+      </c>
+      <c r="D900" t="s">
+        <v>775</v>
+      </c>
+      <c r="E900" t="s">
+        <v>776</v>
+      </c>
+      <c r="F900" t="s">
+        <v>777</v>
+      </c>
+      <c r="G900" t="s">
+        <v>778</v>
+      </c>
+      <c r="H900" t="s">
+        <v>779</v>
+      </c>
+      <c r="I900" t="s">
+        <v>780</v>
+      </c>
+      <c r="J900" t="s">
+        <v>781</v>
+      </c>
+      <c r="K900" t="s">
+        <v>427</v>
+      </c>
+      <c r="L900" t="s">
+        <v>782</v>
+      </c>
+      <c r="M900" t="s">
+        <v>783</v>
+      </c>
+      <c r="N900" t="s">
+        <v>784</v>
+      </c>
+      <c r="O900" t="s">
+        <v>785</v>
+      </c>
+      <c r="P900" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q900" t="s">
+        <v>787</v>
+      </c>
+      <c r="R900" t="s">
+        <v>788</v>
+      </c>
+      <c r="S900" t="s">
+        <v>789</v>
+      </c>
+      <c r="T900" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="901" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
+        <v>772</v>
+      </c>
+      <c r="B901" t="s">
+        <v>773</v>
+      </c>
+      <c r="C901" t="s">
+        <v>774</v>
+      </c>
+      <c r="D901" t="s">
+        <v>775</v>
+      </c>
+      <c r="E901" t="s">
+        <v>776</v>
+      </c>
+      <c r="F901" t="s">
+        <v>777</v>
+      </c>
+      <c r="G901" t="s">
+        <v>778</v>
+      </c>
+      <c r="H901" t="s">
+        <v>779</v>
+      </c>
+      <c r="I901" t="s">
+        <v>780</v>
+      </c>
+      <c r="J901" t="s">
+        <v>781</v>
+      </c>
+      <c r="K901" t="s">
+        <v>427</v>
+      </c>
+      <c r="L901" t="s">
+        <v>782</v>
+      </c>
+      <c r="M901" t="s">
+        <v>783</v>
+      </c>
+      <c r="N901" t="s">
+        <v>784</v>
+      </c>
+      <c r="O901" t="s">
+        <v>785</v>
+      </c>
+      <c r="P901" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q901" t="s">
+        <v>787</v>
+      </c>
+      <c r="R901" t="s">
+        <v>788</v>
+      </c>
+      <c r="S901" t="s">
+        <v>789</v>
+      </c>
+      <c r="T901" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="902" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
+        <v>772</v>
+      </c>
+      <c r="B902" t="s">
+        <v>773</v>
+      </c>
+      <c r="C902" t="s">
+        <v>774</v>
+      </c>
+      <c r="D902" t="s">
+        <v>775</v>
+      </c>
+      <c r="E902" t="s">
+        <v>776</v>
+      </c>
+      <c r="F902" t="s">
+        <v>777</v>
+      </c>
+      <c r="G902" t="s">
+        <v>778</v>
+      </c>
+      <c r="H902" t="s">
+        <v>779</v>
+      </c>
+      <c r="I902" t="s">
+        <v>780</v>
+      </c>
+      <c r="J902" t="s">
+        <v>781</v>
+      </c>
+      <c r="K902" t="s">
+        <v>427</v>
+      </c>
+      <c r="L902" t="s">
+        <v>782</v>
+      </c>
+      <c r="M902" t="s">
+        <v>783</v>
+      </c>
+      <c r="N902" t="s">
+        <v>784</v>
+      </c>
+      <c r="O902" t="s">
+        <v>785</v>
+      </c>
+      <c r="P902" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q902" t="s">
+        <v>787</v>
+      </c>
+      <c r="R902" t="s">
+        <v>788</v>
+      </c>
+      <c r="S902" t="s">
+        <v>789</v>
+      </c>
+      <c r="T902" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="903" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>772</v>
+      </c>
+      <c r="B903" t="s">
+        <v>773</v>
+      </c>
+      <c r="C903" t="s">
+        <v>774</v>
+      </c>
+      <c r="D903" t="s">
+        <v>775</v>
+      </c>
+      <c r="E903" t="s">
+        <v>776</v>
+      </c>
+      <c r="F903" t="s">
+        <v>777</v>
+      </c>
+      <c r="G903" t="s">
+        <v>778</v>
+      </c>
+      <c r="H903" t="s">
+        <v>779</v>
+      </c>
+      <c r="I903" t="s">
+        <v>780</v>
+      </c>
+      <c r="J903" t="s">
+        <v>781</v>
+      </c>
+      <c r="K903" t="s">
+        <v>427</v>
+      </c>
+      <c r="L903" t="s">
+        <v>782</v>
+      </c>
+      <c r="M903" t="s">
+        <v>783</v>
+      </c>
+      <c r="N903" t="s">
+        <v>784</v>
+      </c>
+      <c r="O903" t="s">
+        <v>785</v>
+      </c>
+      <c r="P903" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q903" t="s">
+        <v>787</v>
+      </c>
+      <c r="R903" t="s">
+        <v>788</v>
+      </c>
+      <c r="S903" t="s">
+        <v>789</v>
+      </c>
+      <c r="T903" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="904" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>772</v>
+      </c>
+      <c r="B904" t="s">
+        <v>773</v>
+      </c>
+      <c r="C904" t="s">
+        <v>774</v>
+      </c>
+      <c r="D904" t="s">
+        <v>775</v>
+      </c>
+      <c r="E904" t="s">
+        <v>776</v>
+      </c>
+      <c r="F904" t="s">
+        <v>777</v>
+      </c>
+      <c r="G904" t="s">
+        <v>778</v>
+      </c>
+      <c r="H904" t="s">
+        <v>779</v>
+      </c>
+      <c r="I904" t="s">
+        <v>780</v>
+      </c>
+      <c r="J904" t="s">
+        <v>781</v>
+      </c>
+      <c r="K904" t="s">
+        <v>427</v>
+      </c>
+      <c r="L904" t="s">
+        <v>782</v>
+      </c>
+      <c r="M904" t="s">
+        <v>783</v>
+      </c>
+      <c r="N904" t="s">
+        <v>784</v>
+      </c>
+      <c r="O904" t="s">
+        <v>785</v>
+      </c>
+      <c r="P904" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q904" t="s">
+        <v>787</v>
+      </c>
+      <c r="R904" t="s">
+        <v>788</v>
+      </c>
+      <c r="S904" t="s">
+        <v>789</v>
+      </c>
+      <c r="T904" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="905" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>772</v>
+      </c>
+      <c r="B905" t="s">
+        <v>773</v>
+      </c>
+      <c r="C905" t="s">
+        <v>774</v>
+      </c>
+      <c r="D905" t="s">
+        <v>775</v>
+      </c>
+      <c r="E905" t="s">
+        <v>776</v>
+      </c>
+      <c r="F905" t="s">
+        <v>777</v>
+      </c>
+      <c r="G905" t="s">
+        <v>778</v>
+      </c>
+      <c r="H905" t="s">
+        <v>779</v>
+      </c>
+      <c r="I905" t="s">
+        <v>780</v>
+      </c>
+      <c r="J905" t="s">
+        <v>781</v>
+      </c>
+      <c r="K905" t="s">
+        <v>427</v>
+      </c>
+      <c r="L905" t="s">
+        <v>782</v>
+      </c>
+      <c r="M905" t="s">
+        <v>783</v>
+      </c>
+      <c r="N905" t="s">
+        <v>784</v>
+      </c>
+      <c r="O905" t="s">
+        <v>785</v>
+      </c>
+      <c r="P905" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q905" t="s">
+        <v>787</v>
+      </c>
+      <c r="R905" t="s">
+        <v>788</v>
+      </c>
+      <c r="S905" t="s">
+        <v>789</v>
+      </c>
+      <c r="T905" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="906" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>772</v>
+      </c>
+      <c r="B906" t="s">
+        <v>773</v>
+      </c>
+      <c r="C906" t="s">
+        <v>774</v>
+      </c>
+      <c r="D906" t="s">
+        <v>775</v>
+      </c>
+      <c r="E906" t="s">
+        <v>776</v>
+      </c>
+      <c r="F906" t="s">
+        <v>777</v>
+      </c>
+      <c r="G906" t="s">
+        <v>778</v>
+      </c>
+      <c r="H906" t="s">
+        <v>779</v>
+      </c>
+      <c r="I906" t="s">
+        <v>780</v>
+      </c>
+      <c r="J906" t="s">
+        <v>781</v>
+      </c>
+      <c r="K906" t="s">
+        <v>427</v>
+      </c>
+      <c r="L906" t="s">
+        <v>782</v>
+      </c>
+      <c r="M906" t="s">
+        <v>783</v>
+      </c>
+      <c r="N906" t="s">
+        <v>784</v>
+      </c>
+      <c r="O906" t="s">
+        <v>785</v>
+      </c>
+      <c r="P906" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q906" t="s">
+        <v>787</v>
+      </c>
+      <c r="R906" t="s">
+        <v>788</v>
+      </c>
+      <c r="S906" t="s">
+        <v>789</v>
+      </c>
+      <c r="T906" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="907" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>772</v>
+      </c>
+      <c r="B907" t="s">
+        <v>773</v>
+      </c>
+      <c r="C907" t="s">
+        <v>774</v>
+      </c>
+      <c r="D907" t="s">
+        <v>775</v>
+      </c>
+      <c r="E907" t="s">
+        <v>776</v>
+      </c>
+      <c r="F907" t="s">
+        <v>777</v>
+      </c>
+      <c r="G907" t="s">
+        <v>778</v>
+      </c>
+      <c r="H907" t="s">
+        <v>779</v>
+      </c>
+      <c r="I907" t="s">
+        <v>780</v>
+      </c>
+      <c r="J907" t="s">
+        <v>781</v>
+      </c>
+      <c r="K907" t="s">
+        <v>427</v>
+      </c>
+      <c r="L907" t="s">
+        <v>782</v>
+      </c>
+      <c r="M907" t="s">
+        <v>783</v>
+      </c>
+      <c r="N907" t="s">
+        <v>784</v>
+      </c>
+      <c r="O907" t="s">
+        <v>785</v>
+      </c>
+      <c r="P907" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q907" t="s">
+        <v>787</v>
+      </c>
+      <c r="R907" t="s">
+        <v>788</v>
+      </c>
+      <c r="S907" t="s">
+        <v>789</v>
+      </c>
+      <c r="T907" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="908" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>772</v>
+      </c>
+      <c r="B908" t="s">
+        <v>773</v>
+      </c>
+      <c r="C908" t="s">
+        <v>774</v>
+      </c>
+      <c r="D908" t="s">
+        <v>775</v>
+      </c>
+      <c r="E908" t="s">
+        <v>776</v>
+      </c>
+      <c r="F908" t="s">
+        <v>777</v>
+      </c>
+      <c r="G908" t="s">
+        <v>778</v>
+      </c>
+      <c r="H908" t="s">
+        <v>779</v>
+      </c>
+      <c r="I908" t="s">
+        <v>780</v>
+      </c>
+      <c r="J908" t="s">
+        <v>781</v>
+      </c>
+      <c r="K908" t="s">
+        <v>427</v>
+      </c>
+      <c r="L908" t="s">
+        <v>782</v>
+      </c>
+      <c r="M908" t="s">
+        <v>783</v>
+      </c>
+      <c r="N908" t="s">
+        <v>784</v>
+      </c>
+      <c r="O908" t="s">
+        <v>785</v>
+      </c>
+      <c r="P908" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q908" t="s">
+        <v>787</v>
+      </c>
+      <c r="R908" t="s">
+        <v>788</v>
+      </c>
+      <c r="S908" t="s">
+        <v>789</v>
+      </c>
+      <c r="T908" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="909" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>772</v>
+      </c>
+      <c r="B909" t="s">
+        <v>773</v>
+      </c>
+      <c r="C909" t="s">
+        <v>774</v>
+      </c>
+      <c r="D909" t="s">
+        <v>775</v>
+      </c>
+      <c r="E909" t="s">
+        <v>776</v>
+      </c>
+      <c r="F909" t="s">
+        <v>777</v>
+      </c>
+      <c r="G909" t="s">
+        <v>778</v>
+      </c>
+      <c r="H909" t="s">
+        <v>779</v>
+      </c>
+      <c r="I909" t="s">
+        <v>780</v>
+      </c>
+      <c r="J909" t="s">
+        <v>781</v>
+      </c>
+      <c r="K909" t="s">
+        <v>427</v>
+      </c>
+      <c r="L909" t="s">
+        <v>782</v>
+      </c>
+      <c r="M909" t="s">
+        <v>783</v>
+      </c>
+      <c r="N909" t="s">
+        <v>784</v>
+      </c>
+      <c r="O909" t="s">
+        <v>785</v>
+      </c>
+      <c r="P909" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q909" t="s">
+        <v>787</v>
+      </c>
+      <c r="R909" t="s">
+        <v>788</v>
+      </c>
+      <c r="S909" t="s">
+        <v>789</v>
+      </c>
+      <c r="T909" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="910" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>772</v>
+      </c>
+      <c r="B910" t="s">
+        <v>773</v>
+      </c>
+      <c r="C910" t="s">
+        <v>774</v>
+      </c>
+      <c r="D910" t="s">
+        <v>775</v>
+      </c>
+      <c r="E910" t="s">
+        <v>776</v>
+      </c>
+      <c r="F910" t="s">
+        <v>777</v>
+      </c>
+      <c r="G910" t="s">
+        <v>778</v>
+      </c>
+      <c r="H910" t="s">
+        <v>779</v>
+      </c>
+      <c r="I910" t="s">
+        <v>780</v>
+      </c>
+      <c r="J910" t="s">
+        <v>781</v>
+      </c>
+      <c r="K910" t="s">
+        <v>427</v>
+      </c>
+      <c r="L910" t="s">
+        <v>782</v>
+      </c>
+      <c r="M910" t="s">
+        <v>783</v>
+      </c>
+      <c r="N910" t="s">
+        <v>784</v>
+      </c>
+      <c r="O910" t="s">
+        <v>785</v>
+      </c>
+      <c r="P910" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q910" t="s">
+        <v>787</v>
+      </c>
+      <c r="R910" t="s">
+        <v>788</v>
+      </c>
+      <c r="S910" t="s">
+        <v>789</v>
+      </c>
+      <c r="T910" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="911" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>772</v>
+      </c>
+      <c r="B911" t="s">
+        <v>773</v>
+      </c>
+      <c r="C911" t="s">
+        <v>774</v>
+      </c>
+      <c r="D911" t="s">
+        <v>775</v>
+      </c>
+      <c r="E911" t="s">
+        <v>776</v>
+      </c>
+      <c r="F911" t="s">
+        <v>777</v>
+      </c>
+      <c r="G911" t="s">
+        <v>778</v>
+      </c>
+      <c r="H911" t="s">
+        <v>779</v>
+      </c>
+      <c r="I911" t="s">
+        <v>780</v>
+      </c>
+      <c r="J911" t="s">
+        <v>781</v>
+      </c>
+      <c r="K911" t="s">
+        <v>427</v>
+      </c>
+      <c r="L911" t="s">
+        <v>782</v>
+      </c>
+      <c r="M911" t="s">
+        <v>783</v>
+      </c>
+      <c r="N911" t="s">
+        <v>784</v>
+      </c>
+      <c r="O911" t="s">
+        <v>785</v>
+      </c>
+      <c r="P911" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q911" t="s">
+        <v>787</v>
+      </c>
+      <c r="R911" t="s">
+        <v>788</v>
+      </c>
+      <c r="S911" t="s">
+        <v>789</v>
+      </c>
+      <c r="T911" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="914" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>791</v>
+      </c>
+      <c r="B914" t="s">
+        <v>792</v>
+      </c>
+      <c r="C914" t="s">
+        <v>793</v>
+      </c>
+      <c r="D914" t="s">
+        <v>794</v>
+      </c>
+      <c r="E914" t="s">
+        <v>795</v>
+      </c>
+      <c r="F914" t="s">
+        <v>796</v>
+      </c>
+      <c r="G914" t="s">
+        <v>797</v>
+      </c>
+      <c r="H914" t="s">
+        <v>798</v>
+      </c>
+      <c r="I914" t="s">
+        <v>799</v>
+      </c>
+      <c r="J914" t="s">
+        <v>800</v>
+      </c>
+      <c r="K914" t="s">
+        <v>801</v>
+      </c>
+      <c r="L914" t="s">
+        <v>802</v>
+      </c>
+      <c r="M914" t="s">
+        <v>803</v>
+      </c>
+      <c r="N914" t="s">
+        <v>804</v>
+      </c>
+      <c r="O914" t="s">
+        <v>805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
them sap xep mang cau truc,having sql...
</commit_message>
<xml_diff>
--- a/NOTE/new words.xlsx
+++ b/NOTE/new words.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16371" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16651" uniqueCount="826">
   <si>
     <t>inner: ben trong</t>
   </si>
@@ -2442,6 +2442,66 @@
   </si>
   <si>
     <t>filtration loc</t>
+  </si>
+  <si>
+    <t>accuracy chinh xac</t>
+  </si>
+  <si>
+    <t>acceptable co the chap nhan duoc</t>
+  </si>
+  <si>
+    <t>precise chinh xac</t>
+  </si>
+  <si>
+    <t>revelant thich hop co lien quan</t>
+  </si>
+  <si>
+    <t>inpiration su cam hung</t>
+  </si>
+  <si>
+    <t>intersection giao diem</t>
+  </si>
+  <si>
+    <t>respective tuong ung</t>
+  </si>
+  <si>
+    <t>schema luoc do</t>
+  </si>
+  <si>
+    <t>rigid cung</t>
+  </si>
+  <si>
+    <t>alternative su thay the</t>
+  </si>
+  <si>
+    <t>beam trum</t>
+  </si>
+  <si>
+    <t>inertia quan tinh</t>
+  </si>
+  <si>
+    <t>noticeable de nhan thay</t>
+  </si>
+  <si>
+    <t>prediction su tien doan</t>
+  </si>
+  <si>
+    <t>quantity so luong</t>
+  </si>
+  <si>
+    <t>establish thiet lap</t>
+  </si>
+  <si>
+    <t>permanent vinh vien</t>
+  </si>
+  <si>
+    <t>diverse nhieu loai</t>
+  </si>
+  <si>
+    <t>shape hinh dang</t>
+  </si>
+  <si>
+    <t>virtual ao</t>
   </si>
 </sst>
 </file>
@@ -2827,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V927"/>
+  <dimension ref="A1:V943"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M910" workbookViewId="0">
-      <selection activeCell="P927" sqref="P927"/>
+    <sheetView tabSelected="1" topLeftCell="Q925" workbookViewId="0">
+      <selection activeCell="U943" sqref="U943"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53670,6 +53730,874 @@
       </c>
       <c r="O927" t="s">
         <v>805</v>
+      </c>
+    </row>
+    <row r="930" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>806</v>
+      </c>
+      <c r="B930" t="s">
+        <v>807</v>
+      </c>
+      <c r="C930" t="s">
+        <v>808</v>
+      </c>
+      <c r="D930" t="s">
+        <v>809</v>
+      </c>
+      <c r="E930" t="s">
+        <v>810</v>
+      </c>
+      <c r="F930" t="s">
+        <v>811</v>
+      </c>
+      <c r="G930" t="s">
+        <v>812</v>
+      </c>
+      <c r="H930" t="s">
+        <v>813</v>
+      </c>
+      <c r="I930" t="s">
+        <v>814</v>
+      </c>
+      <c r="J930" t="s">
+        <v>815</v>
+      </c>
+      <c r="K930" t="s">
+        <v>816</v>
+      </c>
+      <c r="L930" t="s">
+        <v>817</v>
+      </c>
+      <c r="M930" t="s">
+        <v>818</v>
+      </c>
+      <c r="N930" t="s">
+        <v>819</v>
+      </c>
+      <c r="O930" t="s">
+        <v>820</v>
+      </c>
+      <c r="P930" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q930" t="s">
+        <v>822</v>
+      </c>
+      <c r="R930" t="s">
+        <v>823</v>
+      </c>
+      <c r="S930" t="s">
+        <v>824</v>
+      </c>
+      <c r="T930" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="931" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A931" t="s">
+        <v>806</v>
+      </c>
+      <c r="B931" t="s">
+        <v>807</v>
+      </c>
+      <c r="C931" t="s">
+        <v>808</v>
+      </c>
+      <c r="D931" t="s">
+        <v>809</v>
+      </c>
+      <c r="E931" t="s">
+        <v>810</v>
+      </c>
+      <c r="F931" t="s">
+        <v>811</v>
+      </c>
+      <c r="G931" t="s">
+        <v>812</v>
+      </c>
+      <c r="H931" t="s">
+        <v>813</v>
+      </c>
+      <c r="I931" t="s">
+        <v>814</v>
+      </c>
+      <c r="J931" t="s">
+        <v>815</v>
+      </c>
+      <c r="K931" t="s">
+        <v>816</v>
+      </c>
+      <c r="L931" t="s">
+        <v>817</v>
+      </c>
+      <c r="M931" t="s">
+        <v>818</v>
+      </c>
+      <c r="N931" t="s">
+        <v>819</v>
+      </c>
+      <c r="O931" t="s">
+        <v>820</v>
+      </c>
+      <c r="P931" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q931" t="s">
+        <v>822</v>
+      </c>
+      <c r="R931" t="s">
+        <v>823</v>
+      </c>
+      <c r="S931" t="s">
+        <v>824</v>
+      </c>
+      <c r="T931" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="932" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A932" t="s">
+        <v>806</v>
+      </c>
+      <c r="B932" t="s">
+        <v>807</v>
+      </c>
+      <c r="C932" t="s">
+        <v>808</v>
+      </c>
+      <c r="D932" t="s">
+        <v>809</v>
+      </c>
+      <c r="E932" t="s">
+        <v>810</v>
+      </c>
+      <c r="F932" t="s">
+        <v>811</v>
+      </c>
+      <c r="G932" t="s">
+        <v>812</v>
+      </c>
+      <c r="H932" t="s">
+        <v>813</v>
+      </c>
+      <c r="I932" t="s">
+        <v>814</v>
+      </c>
+      <c r="J932" t="s">
+        <v>815</v>
+      </c>
+      <c r="K932" t="s">
+        <v>816</v>
+      </c>
+      <c r="L932" t="s">
+        <v>817</v>
+      </c>
+      <c r="M932" t="s">
+        <v>818</v>
+      </c>
+      <c r="N932" t="s">
+        <v>819</v>
+      </c>
+      <c r="O932" t="s">
+        <v>820</v>
+      </c>
+      <c r="P932" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q932" t="s">
+        <v>822</v>
+      </c>
+      <c r="R932" t="s">
+        <v>823</v>
+      </c>
+      <c r="S932" t="s">
+        <v>824</v>
+      </c>
+      <c r="T932" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="933" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>806</v>
+      </c>
+      <c r="B933" t="s">
+        <v>807</v>
+      </c>
+      <c r="C933" t="s">
+        <v>808</v>
+      </c>
+      <c r="D933" t="s">
+        <v>809</v>
+      </c>
+      <c r="E933" t="s">
+        <v>810</v>
+      </c>
+      <c r="F933" t="s">
+        <v>811</v>
+      </c>
+      <c r="G933" t="s">
+        <v>812</v>
+      </c>
+      <c r="H933" t="s">
+        <v>813</v>
+      </c>
+      <c r="I933" t="s">
+        <v>814</v>
+      </c>
+      <c r="J933" t="s">
+        <v>815</v>
+      </c>
+      <c r="K933" t="s">
+        <v>816</v>
+      </c>
+      <c r="L933" t="s">
+        <v>817</v>
+      </c>
+      <c r="M933" t="s">
+        <v>818</v>
+      </c>
+      <c r="N933" t="s">
+        <v>819</v>
+      </c>
+      <c r="O933" t="s">
+        <v>820</v>
+      </c>
+      <c r="P933" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q933" t="s">
+        <v>822</v>
+      </c>
+      <c r="R933" t="s">
+        <v>823</v>
+      </c>
+      <c r="S933" t="s">
+        <v>824</v>
+      </c>
+      <c r="T933" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="934" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A934" t="s">
+        <v>806</v>
+      </c>
+      <c r="B934" t="s">
+        <v>807</v>
+      </c>
+      <c r="C934" t="s">
+        <v>808</v>
+      </c>
+      <c r="D934" t="s">
+        <v>809</v>
+      </c>
+      <c r="E934" t="s">
+        <v>810</v>
+      </c>
+      <c r="F934" t="s">
+        <v>811</v>
+      </c>
+      <c r="G934" t="s">
+        <v>812</v>
+      </c>
+      <c r="H934" t="s">
+        <v>813</v>
+      </c>
+      <c r="I934" t="s">
+        <v>814</v>
+      </c>
+      <c r="J934" t="s">
+        <v>815</v>
+      </c>
+      <c r="K934" t="s">
+        <v>816</v>
+      </c>
+      <c r="L934" t="s">
+        <v>817</v>
+      </c>
+      <c r="M934" t="s">
+        <v>818</v>
+      </c>
+      <c r="N934" t="s">
+        <v>819</v>
+      </c>
+      <c r="O934" t="s">
+        <v>820</v>
+      </c>
+      <c r="P934" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q934" t="s">
+        <v>822</v>
+      </c>
+      <c r="R934" t="s">
+        <v>823</v>
+      </c>
+      <c r="S934" t="s">
+        <v>824</v>
+      </c>
+      <c r="T934" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="935" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A935" t="s">
+        <v>806</v>
+      </c>
+      <c r="B935" t="s">
+        <v>807</v>
+      </c>
+      <c r="C935" t="s">
+        <v>808</v>
+      </c>
+      <c r="D935" t="s">
+        <v>809</v>
+      </c>
+      <c r="E935" t="s">
+        <v>810</v>
+      </c>
+      <c r="F935" t="s">
+        <v>811</v>
+      </c>
+      <c r="G935" t="s">
+        <v>812</v>
+      </c>
+      <c r="H935" t="s">
+        <v>813</v>
+      </c>
+      <c r="I935" t="s">
+        <v>814</v>
+      </c>
+      <c r="J935" t="s">
+        <v>815</v>
+      </c>
+      <c r="K935" t="s">
+        <v>816</v>
+      </c>
+      <c r="L935" t="s">
+        <v>817</v>
+      </c>
+      <c r="M935" t="s">
+        <v>818</v>
+      </c>
+      <c r="N935" t="s">
+        <v>819</v>
+      </c>
+      <c r="O935" t="s">
+        <v>820</v>
+      </c>
+      <c r="P935" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q935" t="s">
+        <v>822</v>
+      </c>
+      <c r="R935" t="s">
+        <v>823</v>
+      </c>
+      <c r="S935" t="s">
+        <v>824</v>
+      </c>
+      <c r="T935" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="936" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A936" t="s">
+        <v>806</v>
+      </c>
+      <c r="B936" t="s">
+        <v>807</v>
+      </c>
+      <c r="C936" t="s">
+        <v>808</v>
+      </c>
+      <c r="D936" t="s">
+        <v>809</v>
+      </c>
+      <c r="E936" t="s">
+        <v>810</v>
+      </c>
+      <c r="F936" t="s">
+        <v>811</v>
+      </c>
+      <c r="G936" t="s">
+        <v>812</v>
+      </c>
+      <c r="H936" t="s">
+        <v>813</v>
+      </c>
+      <c r="I936" t="s">
+        <v>814</v>
+      </c>
+      <c r="J936" t="s">
+        <v>815</v>
+      </c>
+      <c r="K936" t="s">
+        <v>816</v>
+      </c>
+      <c r="L936" t="s">
+        <v>817</v>
+      </c>
+      <c r="M936" t="s">
+        <v>818</v>
+      </c>
+      <c r="N936" t="s">
+        <v>819</v>
+      </c>
+      <c r="O936" t="s">
+        <v>820</v>
+      </c>
+      <c r="P936" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q936" t="s">
+        <v>822</v>
+      </c>
+      <c r="R936" t="s">
+        <v>823</v>
+      </c>
+      <c r="S936" t="s">
+        <v>824</v>
+      </c>
+      <c r="T936" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="937" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>806</v>
+      </c>
+      <c r="B937" t="s">
+        <v>807</v>
+      </c>
+      <c r="C937" t="s">
+        <v>808</v>
+      </c>
+      <c r="D937" t="s">
+        <v>809</v>
+      </c>
+      <c r="E937" t="s">
+        <v>810</v>
+      </c>
+      <c r="F937" t="s">
+        <v>811</v>
+      </c>
+      <c r="G937" t="s">
+        <v>812</v>
+      </c>
+      <c r="H937" t="s">
+        <v>813</v>
+      </c>
+      <c r="I937" t="s">
+        <v>814</v>
+      </c>
+      <c r="J937" t="s">
+        <v>815</v>
+      </c>
+      <c r="K937" t="s">
+        <v>816</v>
+      </c>
+      <c r="L937" t="s">
+        <v>817</v>
+      </c>
+      <c r="M937" t="s">
+        <v>818</v>
+      </c>
+      <c r="N937" t="s">
+        <v>819</v>
+      </c>
+      <c r="O937" t="s">
+        <v>820</v>
+      </c>
+      <c r="P937" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q937" t="s">
+        <v>822</v>
+      </c>
+      <c r="R937" t="s">
+        <v>823</v>
+      </c>
+      <c r="S937" t="s">
+        <v>824</v>
+      </c>
+      <c r="T937" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="938" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>806</v>
+      </c>
+      <c r="B938" t="s">
+        <v>807</v>
+      </c>
+      <c r="C938" t="s">
+        <v>808</v>
+      </c>
+      <c r="D938" t="s">
+        <v>809</v>
+      </c>
+      <c r="E938" t="s">
+        <v>810</v>
+      </c>
+      <c r="F938" t="s">
+        <v>811</v>
+      </c>
+      <c r="G938" t="s">
+        <v>812</v>
+      </c>
+      <c r="H938" t="s">
+        <v>813</v>
+      </c>
+      <c r="I938" t="s">
+        <v>814</v>
+      </c>
+      <c r="J938" t="s">
+        <v>815</v>
+      </c>
+      <c r="K938" t="s">
+        <v>816</v>
+      </c>
+      <c r="L938" t="s">
+        <v>817</v>
+      </c>
+      <c r="M938" t="s">
+        <v>818</v>
+      </c>
+      <c r="N938" t="s">
+        <v>819</v>
+      </c>
+      <c r="O938" t="s">
+        <v>820</v>
+      </c>
+      <c r="P938" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q938" t="s">
+        <v>822</v>
+      </c>
+      <c r="R938" t="s">
+        <v>823</v>
+      </c>
+      <c r="S938" t="s">
+        <v>824</v>
+      </c>
+      <c r="T938" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="939" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>806</v>
+      </c>
+      <c r="B939" t="s">
+        <v>807</v>
+      </c>
+      <c r="C939" t="s">
+        <v>808</v>
+      </c>
+      <c r="D939" t="s">
+        <v>809</v>
+      </c>
+      <c r="E939" t="s">
+        <v>810</v>
+      </c>
+      <c r="F939" t="s">
+        <v>811</v>
+      </c>
+      <c r="G939" t="s">
+        <v>812</v>
+      </c>
+      <c r="H939" t="s">
+        <v>813</v>
+      </c>
+      <c r="I939" t="s">
+        <v>814</v>
+      </c>
+      <c r="J939" t="s">
+        <v>815</v>
+      </c>
+      <c r="K939" t="s">
+        <v>816</v>
+      </c>
+      <c r="L939" t="s">
+        <v>817</v>
+      </c>
+      <c r="M939" t="s">
+        <v>818</v>
+      </c>
+      <c r="N939" t="s">
+        <v>819</v>
+      </c>
+      <c r="O939" t="s">
+        <v>820</v>
+      </c>
+      <c r="P939" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q939" t="s">
+        <v>822</v>
+      </c>
+      <c r="R939" t="s">
+        <v>823</v>
+      </c>
+      <c r="S939" t="s">
+        <v>824</v>
+      </c>
+      <c r="T939" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="940" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>806</v>
+      </c>
+      <c r="B940" t="s">
+        <v>807</v>
+      </c>
+      <c r="C940" t="s">
+        <v>808</v>
+      </c>
+      <c r="D940" t="s">
+        <v>809</v>
+      </c>
+      <c r="E940" t="s">
+        <v>810</v>
+      </c>
+      <c r="F940" t="s">
+        <v>811</v>
+      </c>
+      <c r="G940" t="s">
+        <v>812</v>
+      </c>
+      <c r="H940" t="s">
+        <v>813</v>
+      </c>
+      <c r="I940" t="s">
+        <v>814</v>
+      </c>
+      <c r="J940" t="s">
+        <v>815</v>
+      </c>
+      <c r="K940" t="s">
+        <v>816</v>
+      </c>
+      <c r="L940" t="s">
+        <v>817</v>
+      </c>
+      <c r="M940" t="s">
+        <v>818</v>
+      </c>
+      <c r="N940" t="s">
+        <v>819</v>
+      </c>
+      <c r="O940" t="s">
+        <v>820</v>
+      </c>
+      <c r="P940" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q940" t="s">
+        <v>822</v>
+      </c>
+      <c r="R940" t="s">
+        <v>823</v>
+      </c>
+      <c r="S940" t="s">
+        <v>824</v>
+      </c>
+      <c r="T940" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="941" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>806</v>
+      </c>
+      <c r="B941" t="s">
+        <v>807</v>
+      </c>
+      <c r="C941" t="s">
+        <v>808</v>
+      </c>
+      <c r="D941" t="s">
+        <v>809</v>
+      </c>
+      <c r="E941" t="s">
+        <v>810</v>
+      </c>
+      <c r="F941" t="s">
+        <v>811</v>
+      </c>
+      <c r="G941" t="s">
+        <v>812</v>
+      </c>
+      <c r="H941" t="s">
+        <v>813</v>
+      </c>
+      <c r="I941" t="s">
+        <v>814</v>
+      </c>
+      <c r="J941" t="s">
+        <v>815</v>
+      </c>
+      <c r="K941" t="s">
+        <v>816</v>
+      </c>
+      <c r="L941" t="s">
+        <v>817</v>
+      </c>
+      <c r="M941" t="s">
+        <v>818</v>
+      </c>
+      <c r="N941" t="s">
+        <v>819</v>
+      </c>
+      <c r="O941" t="s">
+        <v>820</v>
+      </c>
+      <c r="P941" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q941" t="s">
+        <v>822</v>
+      </c>
+      <c r="R941" t="s">
+        <v>823</v>
+      </c>
+      <c r="S941" t="s">
+        <v>824</v>
+      </c>
+      <c r="T941" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="942" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>806</v>
+      </c>
+      <c r="B942" t="s">
+        <v>807</v>
+      </c>
+      <c r="C942" t="s">
+        <v>808</v>
+      </c>
+      <c r="D942" t="s">
+        <v>809</v>
+      </c>
+      <c r="E942" t="s">
+        <v>810</v>
+      </c>
+      <c r="F942" t="s">
+        <v>811</v>
+      </c>
+      <c r="G942" t="s">
+        <v>812</v>
+      </c>
+      <c r="H942" t="s">
+        <v>813</v>
+      </c>
+      <c r="I942" t="s">
+        <v>814</v>
+      </c>
+      <c r="J942" t="s">
+        <v>815</v>
+      </c>
+      <c r="K942" t="s">
+        <v>816</v>
+      </c>
+      <c r="L942" t="s">
+        <v>817</v>
+      </c>
+      <c r="M942" t="s">
+        <v>818</v>
+      </c>
+      <c r="N942" t="s">
+        <v>819</v>
+      </c>
+      <c r="O942" t="s">
+        <v>820</v>
+      </c>
+      <c r="P942" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q942" t="s">
+        <v>822</v>
+      </c>
+      <c r="R942" t="s">
+        <v>823</v>
+      </c>
+      <c r="S942" t="s">
+        <v>824</v>
+      </c>
+      <c r="T942" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="943" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>806</v>
+      </c>
+      <c r="B943" t="s">
+        <v>807</v>
+      </c>
+      <c r="C943" t="s">
+        <v>808</v>
+      </c>
+      <c r="D943" t="s">
+        <v>809</v>
+      </c>
+      <c r="E943" t="s">
+        <v>810</v>
+      </c>
+      <c r="F943" t="s">
+        <v>811</v>
+      </c>
+      <c r="G943" t="s">
+        <v>812</v>
+      </c>
+      <c r="H943" t="s">
+        <v>813</v>
+      </c>
+      <c r="I943" t="s">
+        <v>814</v>
+      </c>
+      <c r="J943" t="s">
+        <v>815</v>
+      </c>
+      <c r="K943" t="s">
+        <v>816</v>
+      </c>
+      <c r="L943" t="s">
+        <v>817</v>
+      </c>
+      <c r="M943" t="s">
+        <v>818</v>
+      </c>
+      <c r="N943" t="s">
+        <v>819</v>
+      </c>
+      <c r="O943" t="s">
+        <v>820</v>
+      </c>
+      <c r="P943" t="s">
+        <v>821</v>
+      </c>
+      <c r="Q943" t="s">
+        <v>822</v>
+      </c>
+      <c r="R943" t="s">
+        <v>823</v>
+      </c>
+      <c r="S943" t="s">
+        <v>824</v>
+      </c>
+      <c r="T943" t="s">
+        <v>825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>